<commit_message>
Actualización automática desde WSL
</commit_message>
<xml_diff>
--- a/datos_dropcontrol/2025-08-05.xlsx
+++ b/datos_dropcontrol/2025-08-05.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,7 +815,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45874.41689232497</v>
+        <v>45874.41689232639</v>
       </c>
       <c r="B12" t="n">
         <v>2025</v>
@@ -846,6 +846,78 @@
       <c r="J12" t="inlineStr">
         <is>
           <t>10:00:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45874.43292002315</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C13" t="n">
+        <v>19</v>
+      </c>
+      <c r="D13" t="n">
+        <v>16.17</v>
+      </c>
+      <c r="E13" t="n">
+        <v>89.66</v>
+      </c>
+      <c r="F13" t="n">
+        <v>499.22</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9.34</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ESE</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>10:23:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45874.44107065022</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C14" t="n">
+        <v>19</v>
+      </c>
+      <c r="D14" t="n">
+        <v>17.22</v>
+      </c>
+      <c r="E14" t="n">
+        <v>85.18000000000001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>335.74</v>
+      </c>
+      <c r="G14" t="n">
+        <v>9.16</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ESE</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>10:35:08</t>
         </is>
       </c>
     </row>

</xml_diff>